<commit_message>
Cambio  a versio PRD 2023-06-22 Ajuste a conceptos de Pago
</commit_message>
<xml_diff>
--- a/Script/Dataframes/df_Constancia.xlsx
+++ b/Script/Dataframes/df_Constancia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia agrol  diciembre 2022.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia agrol  diciembre 2022.pdf</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia bricks febrero 2023.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia bricks febrero 2023.pdf</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia codigo a enero 2023.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia codigo a enero 2023.pdf</t>
         </is>
       </c>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia cuadras asesores diciembre 2022.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia cuadras asesores diciembre 2022.pdf</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia desoflex 19-03-2020.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia desoflex 19-03-2020.pdf</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia diseños luna 10-01-23.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia diseños luna 10-01-23.pdf</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\Constancia Interexporta MARZO 2023.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\Constancia Interexporta MARZO 2023.pdf</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia jose luis zarate losa 19-01-23.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia jose luis zarate losa 19-01-23.pdf</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia moises mercado torres 03-11-22.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia moises mercado torres 03-11-22.pdf</t>
         </is>
       </c>
     </row>
@@ -948,7 +948,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia monica alejandra zarate losa  22-02-23.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia monica alejandra zarate losa  22-02-23.pdf</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia pascual ibarra 23-01-23.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia pascual ibarra 23-01-23.pdf</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia rigoberto mora 10-01-23.pdf</t>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia rigoberto mora 10-01-23.pdf</t>
         </is>
       </c>
     </row>
@@ -1070,48 +1070,101 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAJR890708VB7 </t>
+          <t xml:space="preserve">MOAR741018D36 </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JAJR890708MJCRRS06 </t>
+          <t xml:space="preserve"> MOAR741018HJCRLG02 </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JAJR890708MJCRRS06 </t>
+          <t xml:space="preserve"> MOAR741018HJCRLG02 </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JAUREGUI </t>
+          <t xml:space="preserve"> MORA </t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JAUREGUI </t>
+          <t xml:space="preserve"> ALVAREZ </t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 01DEJUNIODE1996</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> REACTIVADO </t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Regímenes:   Régimen Fecha Inicio Fecha Fin Régimen de Ingresos por Dividendos (socios y accionistas) 01/01/2017 Régimen de las Personas Físicas con Actividades Empresariales y Profesionales 01/01/2019 Obligaciones</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia rigoberto mora ENERO 2023.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Constancia</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JAJR890708VB7 </t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JAJR890708MJCRRS06 </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JAJR890708MJCRRS06 </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JAUREGUI </t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JAUREGUI </t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 04DEOCTUBRE DE2013</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t xml:space="preserve"> ACTIVO </t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Regímenes:   Régimen Fecha Inicio Fecha Fin Régimen de Incorporación Fiscal 01/08/2014 Obligaciones</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\constancia rosa karmin jauregui 16-02-23.pdf</t>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>C:\Users\victo\Documents\Proyectos\Automatizacion-Cuadras\PDF\PDF\constancia rosa karmin jauregui 16-02-23.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>